<commit_message>
First working report of addressLIst
</commit_message>
<xml_diff>
--- a/src/dataloaddump/param/ModelFieldMapper.xlsx
+++ b/src/dataloaddump/param/ModelFieldMapper.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,10 +483,6 @@
           <t>GeographicalUnitId</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
       <c r="H2" t="b">
         <v>1</v>
       </c>
@@ -507,10 +503,6 @@
           <t>GeographicalUnitCategory</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
       <c r="H3" t="b">
         <v>1</v>
       </c>
@@ -531,10 +523,6 @@
           <t>HierarchyLevel</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
       <c r="H4" t="b">
         <v>1</v>
       </c>
@@ -555,10 +543,6 @@
           <t>geographicalunit_ptr</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
       <c r="H5" t="b">
         <v>1</v>
       </c>
@@ -731,7 +715,6 @@
           <t>IsPartOf</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr">
         <is>
           <t>locations</t>
@@ -803,10 +786,6 @@
           <t>GeographicalUnitId</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
       <c r="H14" t="b">
         <v>1</v>
       </c>
@@ -827,10 +806,6 @@
           <t>GeographicalUnitCategory</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
       <c r="H15" t="b">
         <v>1</v>
       </c>
@@ -856,9 +831,6 @@
           <t>CityName</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
       <c r="H16" t="b">
         <v>0</v>
       </c>
@@ -884,9 +856,6 @@
           <t>CityShortName</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
       <c r="H17" t="b">
         <v>0</v>
       </c>
@@ -907,10 +876,6 @@
           <t>HierarchyLevel</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
       <c r="H18" t="b">
         <v>1</v>
       </c>
@@ -931,7 +896,6 @@
           <t>IsPartOf</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr">
         <is>
           <t>locations</t>
@@ -967,11 +931,199 @@
           <t>geographicalunit_ptr</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
       <c r="H20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>locations</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Address</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>City</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>locations</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>City</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>GeographicalUnitName</t>
+        </is>
+      </c>
+      <c r="H21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>locations</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Address</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Country</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>locations</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Country</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>GeographicalUnitName</t>
+        </is>
+      </c>
+      <c r="H22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>locations</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Address</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>created_by</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>auth</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>user</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>username</t>
+        </is>
+      </c>
+      <c r="H23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>locations</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Address</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>updated_by</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>auth</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>user</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>username</t>
+        </is>
+      </c>
+      <c r="H24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>locations</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Address</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>locations</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Address</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>created</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>